<commit_message>
Initiating create engagement button
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>isbtnUpdate</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Imprimer les listes filtrées</t>
+  </si>
+  <si>
+    <t>Loguer avec le matricule au lieu de l'email</t>
   </si>
 </sst>
 </file>
@@ -687,10 +690,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,10 +702,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C1" t="s">
@@ -718,116 +721,122 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+    <row r="19" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1)Finishing create eng button component. 2) Updating home view to solve infinite loop bug when rendering
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>isbtnUpdate</t>
   </si>
@@ -193,6 +193,15 @@
   </si>
   <si>
     <t>Loguer avec le matricule au lieu de l'email</t>
+  </si>
+  <si>
+    <t>Création engagement</t>
+  </si>
+  <si>
+    <t>Tous les champs doivent être renseignés</t>
+  </si>
+  <si>
+    <t>Le montant de création doit être &gt; 0 et &lt; au solde restant de la ligne</t>
   </si>
 </sst>
 </file>
@@ -690,10 +699,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,108 +744,122 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Start rules on create engagement form
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -701,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
1) Edit create engagement form to add rules 2) remove 'montant_ht' from all enagements forms : apurementcard, apurement creation, imputationcard, imputation creation , engagementcard, engagement creation
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -243,11 +243,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -701,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,12 +822,14 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding rules to engagement creation form
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
   <si>
     <t>isbtnUpdate</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>Le montant de création doit être &gt; 0 et &lt; au solde restant de la ligne</t>
+  </si>
+  <si>
+    <t>Création apurement</t>
+  </si>
+  <si>
+    <t>Création imputation</t>
   </si>
 </sst>
 </file>
@@ -702,10 +708,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,124 +753,136 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="4" t="s">
+    <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit login page to be more presentable
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -711,7 +711,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,9 +748,10 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -767,16 +768,16 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -830,7 +831,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding reason for engagement closing
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -711,7 +711,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +858,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1) Adding Type paiement to apurment 2) Other minor changes
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>isbtnUpdate</t>
   </si>
@@ -174,9 +174,6 @@
   </si>
   <si>
     <t>Ajouter une liste déroulante lorsque l'utilisateur veut clôturer un engagement</t>
-  </si>
-  <si>
-    <t>Ecritures de régularisation</t>
   </si>
   <si>
     <t>Planifier la mise en oeuvre de l'application pour Douala</t>
@@ -249,13 +246,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -708,9 +702,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -741,7 +735,7 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,27 +749,27 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -836,13 +830,13 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -863,28 +857,23 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing unecessary buttons/actions on navbar
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -705,7 +705,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +872,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>